<commit_message>
Tambah lap AP1, security dan perbaiki logika logout
</commit_message>
<xml_diff>
--- a/assets/tpl/rp.xlsx
+++ b/assets/tpl/rp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\smep19\assets\tpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C31D988-9075-4C33-AB20-6E9FE6ABD2C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA830B40-F16E-43E1-BE7F-4B455D2B6697}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="15600" windowHeight="7940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>KABUPATEN</t>
   </si>
@@ -39,9 +39,6 @@
     <t>TAHUN ANGGARAN</t>
   </si>
   <si>
-    <t>NO.</t>
-  </si>
-  <si>
     <t>METODE PENGADAAN</t>
   </si>
   <si>
@@ -82,6 +79,12 @@
   </si>
   <si>
     <t>PPK</t>
+  </si>
+  <si>
+    <t>KODE REK</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -609,25 +612,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="44.26953125" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="10" width="11.08984375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="3" max="3" width="44.26953125" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" customWidth="1"/>
+    <col min="6" max="11" width="11.08984375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -639,8 +643,9 @@
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -652,14 +657,14 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="9"/>
+        <v>7</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -667,14 +672,14 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -682,14 +687,14 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -697,10 +702,10 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -710,28 +715,29 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K7" s="9"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>6</v>
@@ -739,44 +745,48 @@
       <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="15"/>
+      <c r="E8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>2</v>
+      </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.35">
+      <c r="J8" s="15"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="13"/>
+      <c r="F9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="I9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="K9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="13"/>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -789,7 +799,7 @@
       <c r="D10" s="5">
         <v>4</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>5</v>
       </c>
       <c r="F10" s="6">
@@ -807,32 +817,37 @@
       <c r="J10" s="6">
         <v>10</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="6">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="1"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A1:K1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="F8:K8"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="E8:J8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.39370078740157483" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>